<commit_message>
add post on time series
</commit_message>
<xml_diff>
--- a/content/post/extracted/pp_zanzibar.xlsx
+++ b/content/post/extracted/pp_zanzibar.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TAFIRI_1\DSFA\PROJECTS\PFZ\PFZ data\PP 2019\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="132" windowWidth="9996" windowHeight="9996"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -45,10 +50,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Cambria"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -572,6 +576,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -587,39 +594,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -654,7 +661,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -698,166 +705,142 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
@@ -867,14 +850,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -885,7 +868,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>42370</v>
       </c>
@@ -893,10 +876,10 @@
         <v>2003</v>
       </c>
       <c r="C2" s="3">
-        <v>1412.54005872483</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1085.69466560509</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>42370</v>
       </c>
@@ -904,10 +887,10 @@
         <v>2004</v>
       </c>
       <c r="C3" s="3">
-        <v>1163.92649371069</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>708.12015086206895</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>42370</v>
       </c>
@@ -915,10 +898,10 @@
         <v>2005</v>
       </c>
       <c r="C4" s="3">
-        <v>1228.91721854304</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>806.10526842948696</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>42370</v>
       </c>
@@ -926,10 +909,10 @@
         <v>2006</v>
       </c>
       <c r="C5" s="3">
-        <v>1203.91185897435</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>769.17177483974297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>42370</v>
       </c>
@@ -937,10 +920,10 @@
         <v>2007</v>
       </c>
       <c r="C6" s="3">
-        <v>1275.84973144531</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1104.83502155172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>42370</v>
       </c>
@@ -948,10 +931,10 @@
         <v>2008</v>
       </c>
       <c r="C7" s="3">
-        <v>1158.8309948979499</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>724.64460784313701</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>42370</v>
       </c>
@@ -959,10 +942,10 @@
         <v>2009</v>
       </c>
       <c r="C8" s="3">
-        <v>1224.7226821192</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>783.99421672077904</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>42370</v>
       </c>
@@ -970,10 +953,10 @@
         <v>2010</v>
       </c>
       <c r="C9" s="3">
-        <v>1223.94838362068</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>784.39684078467099</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>42370</v>
       </c>
@@ -981,10 +964,10 @@
         <v>2011</v>
       </c>
       <c r="C10" s="3">
-        <v>1193.8122859589</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>856.25496651785704</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>42370</v>
       </c>
@@ -992,10 +975,10 @@
         <v>2012</v>
       </c>
       <c r="C11" s="3">
-        <v>1093.5721460459099</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1045.7999799679401</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>42370</v>
       </c>
@@ -1003,10 +986,10 @@
         <v>2013</v>
       </c>
       <c r="C12" s="3">
-        <v>1161.6798930921</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>952.18709935897402</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>42370</v>
       </c>
@@ -1014,10 +997,10 @@
         <v>2014</v>
       </c>
       <c r="C13" s="3">
-        <v>1011.58102678571</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>771.77933902877703</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>42370</v>
       </c>
@@ -1025,10 +1008,10 @@
         <v>2015</v>
       </c>
       <c r="C14" s="3">
-        <v>1085.1505681818101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>916.56731592465701</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>42370</v>
       </c>
@@ -1036,10 +1019,10 @@
         <v>2016</v>
       </c>
       <c r="C15" s="3">
-        <v>1290.5357142857099</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>788.56097898229996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>42370</v>
       </c>
@@ -1047,10 +1030,10 @@
         <v>2017</v>
       </c>
       <c r="C16" s="3">
-        <v>1339.9083333333299</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>944.82786016949103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>42370</v>
       </c>
@@ -1058,10 +1041,10 @@
         <v>2018</v>
       </c>
       <c r="C17" s="3">
-        <v>1299.7248330152599</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>984.95870535714198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>42401</v>
       </c>
@@ -1069,10 +1052,10 @@
         <v>2003</v>
       </c>
       <c r="C18" s="3">
-        <v>1326.8682709853999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>772.58056640625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>42401</v>
       </c>
@@ -1080,10 +1063,10 @@
         <v>2004</v>
       </c>
       <c r="C19" s="3">
-        <v>1191.62955298013</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>706.53722734899304</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>42401</v>
       </c>
@@ -1091,10 +1074,10 @@
         <v>2005</v>
       </c>
       <c r="C20" s="3">
-        <v>1261.67694256756</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>694.73935231854796</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>42401</v>
       </c>
@@ -1102,10 +1085,10 @@
         <v>2006</v>
       </c>
       <c r="C21" s="3">
-        <v>1148.90183189655</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>766.80372299382702</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>42401</v>
       </c>
@@ -1113,10 +1096,10 @@
         <v>2007</v>
       </c>
       <c r="C22" s="3">
-        <v>1014.47948473282</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>717.719396551724</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>42401</v>
       </c>
@@ -1124,10 +1107,10 @@
         <v>2008</v>
       </c>
       <c r="C23" s="3">
-        <v>1308.1455965908999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>740.87162162162099</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>42401</v>
       </c>
@@ -1135,10 +1118,10 @@
         <v>2009</v>
       </c>
       <c r="C24" s="3">
-        <v>1293</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>707.77996439873402</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>42401</v>
       </c>
@@ -1146,10 +1129,10 @@
         <v>2010</v>
       </c>
       <c r="C25" s="3">
-        <v>1141.4379340277701</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>662.11144301470495</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>42401</v>
       </c>
@@ -1157,10 +1140,10 @@
         <v>2011</v>
       </c>
       <c r="C26" s="3">
-        <v>1201.15384615384</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>826.57663445723597</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>42401</v>
       </c>
@@ -1168,10 +1151,10 @@
         <v>2012</v>
       </c>
       <c r="C27" s="3">
-        <v>1044.95986519607</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>714.65321969696902</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>42401</v>
       </c>
@@ -1179,10 +1162,10 @@
         <v>2013</v>
       </c>
       <c r="C28" s="3">
-        <v>1144.2634892086301</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>826.32307841614897</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>42401</v>
       </c>
@@ -1190,10 +1173,10 @@
         <v>2014</v>
       </c>
       <c r="C29" s="3">
-        <v>862.99079056291396</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>618.70003939075605</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>42401</v>
       </c>
@@ -1201,10 +1184,10 @@
         <v>2015</v>
       </c>
       <c r="C30" s="3">
-        <v>1130.7497902684499</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>694.65173192770999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>42401</v>
       </c>
@@ -1212,10 +1195,10 @@
         <v>2016</v>
       </c>
       <c r="C31" s="3">
-        <v>1014.38057002314</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>838.31770833333303</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>42401</v>
       </c>
@@ -1223,10 +1206,10 @@
         <v>2017</v>
       </c>
       <c r="C32" s="3">
-        <v>1406.5870398773</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>773.59691011235896</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>42401</v>
       </c>
@@ -1234,10 +1217,10 @@
         <v>2018</v>
       </c>
       <c r="C33" s="3">
-        <v>1196.0480840773801</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>714.40359042553098</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>42430</v>
       </c>
@@ -1245,10 +1228,10 @@
         <v>2003</v>
       </c>
       <c r="C34" s="3">
-        <v>1418.2261257763901</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>887.09799494219601</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>42430</v>
       </c>
@@ -1256,10 +1239,10 @@
         <v>2004</v>
       </c>
       <c r="C35" s="3">
-        <v>1218.3545673076901</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>718.16731366459601</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>42430</v>
       </c>
@@ -1267,10 +1250,10 @@
         <v>2005</v>
       </c>
       <c r="C36" s="3">
-        <v>1363.06079727564</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>766.46158030063202</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>42430</v>
       </c>
@@ -1278,10 +1261,10 @@
         <v>2006</v>
       </c>
       <c r="C37" s="3">
-        <v>1218.47575081168</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>681.77963709677397</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>42430</v>
       </c>
@@ -1289,10 +1272,10 @@
         <v>2007</v>
       </c>
       <c r="C38" s="3">
-        <v>1314.04979166666</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>758.45996732026094</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>42430</v>
       </c>
@@ -1300,10 +1283,10 @@
         <v>2008</v>
       </c>
       <c r="C39" s="3">
-        <v>1314.6187913907199</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>689.03733766233699</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>42430</v>
       </c>
@@ -1311,10 +1294,10 @@
         <v>2009</v>
       </c>
       <c r="C40" s="3">
-        <v>1240.5885754870101</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>765.31602822580601</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>42430</v>
       </c>
@@ -1322,10 +1305,10 @@
         <v>2010</v>
       </c>
       <c r="C41" s="3">
-        <v>1367.0793269230701</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>758.47065304487103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>42430</v>
       </c>
@@ -1333,10 +1316,10 @@
         <v>2011</v>
       </c>
       <c r="C42" s="3">
-        <v>1207.30149371069</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>688.24702380952294</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42430</v>
       </c>
@@ -1344,10 +1327,10 @@
         <v>2012</v>
       </c>
       <c r="C43" s="3">
-        <v>1135.953125</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>690.91738281250002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>42430</v>
       </c>
@@ -1355,10 +1338,10 @@
         <v>2013</v>
       </c>
       <c r="C44" s="3">
-        <v>1147.94689941406</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>719.924779647435</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>42430</v>
       </c>
@@ -1366,10 +1349,10 @@
         <v>2014</v>
       </c>
       <c r="C45" s="3">
-        <v>951.22610294117601</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>554.41333705357101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>42430</v>
       </c>
@@ -1377,10 +1360,10 @@
         <v>2015</v>
       </c>
       <c r="C46" s="3">
-        <v>1027.20787584459</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>574.64216549295702</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>42430</v>
       </c>
@@ -1388,10 +1371,10 @@
         <v>2016</v>
       </c>
       <c r="C47" s="3">
-        <v>1303.4330357142801</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>700.65467825443704</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>42430</v>
       </c>
@@ -1399,10 +1382,10 @@
         <v>2017</v>
       </c>
       <c r="C48" s="3">
-        <v>1284.71915849673</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>796.52548462566801</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>42430</v>
       </c>
@@ -1410,10 +1393,10 @@
         <v>2018</v>
       </c>
       <c r="C49" s="3">
-        <v>1367.2666420118301</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>824.67072368420997</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>42461</v>
       </c>
@@ -1421,10 +1404,10 @@
         <v>2003</v>
       </c>
       <c r="C50" s="3">
-        <v>1531.005078125</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>938.74180640243901</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>42461</v>
       </c>
@@ -1432,10 +1415,10 @@
         <v>2004</v>
       </c>
       <c r="C51" s="3">
-        <v>1295.30017006802</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>737.44974512411295</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>42461</v>
       </c>
@@ -1443,10 +1426,10 @@
         <v>2005</v>
       </c>
       <c r="C52" s="3">
-        <v>1365.8090503246699</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>882.538726993865</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>42461</v>
       </c>
@@ -1454,10 +1437,10 @@
         <v>2006</v>
       </c>
       <c r="C53" s="3">
-        <v>1168.7672139830499</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>692.04565746753201</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>42461</v>
       </c>
@@ -1465,10 +1448,10 @@
         <v>2007</v>
       </c>
       <c r="C54" s="3">
-        <v>1391.9359374999999</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>756.83522727272702</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>42461</v>
       </c>
@@ -1476,10 +1459,10 @@
         <v>2008</v>
       </c>
       <c r="C55" s="3">
-        <v>1351.14288651315</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>925.95358187134502</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>42461</v>
       </c>
@@ -1487,10 +1470,10 @@
         <v>2009</v>
       </c>
       <c r="C56" s="3">
-        <v>1341.7806490384601</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>768.50592830882294</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>42461</v>
       </c>
@@ -1498,10 +1481,10 @@
         <v>2010</v>
       </c>
       <c r="C57" s="3">
-        <v>1255.8035130718899</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>794.85214710884304</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>42461</v>
       </c>
@@ -1509,10 +1492,10 @@
         <v>2011</v>
       </c>
       <c r="C58" s="3">
-        <v>1318.5400455298</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>763.51282051281999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>42461</v>
       </c>
@@ -1520,10 +1503,10 @@
         <v>2012</v>
       </c>
       <c r="C59" s="3">
-        <v>1391.64833603896</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>784.80443548387098</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>42461</v>
       </c>
@@ -1531,10 +1514,10 @@
         <v>2013</v>
       </c>
       <c r="C60" s="3">
-        <v>1380.19911858974</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>837.84525602409599</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>42461</v>
       </c>
@@ -1542,10 +1525,10 @@
         <v>2014</v>
       </c>
       <c r="C61" s="3">
-        <v>1242.4226973684199</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>757.56878810975604</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>42461</v>
       </c>
@@ -1553,10 +1536,10 @@
         <v>2015</v>
       </c>
       <c r="C62" s="3">
-        <v>1232.3060064935</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>648.14237132352901</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>42461</v>
       </c>
@@ -1564,10 +1547,10 @@
         <v>2016</v>
       </c>
       <c r="C63" s="3">
-        <v>1293.87594288793</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>751.77677149681494</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>42461</v>
       </c>
@@ -1575,10 +1558,10 @@
         <v>2017</v>
       </c>
       <c r="C64" s="3">
-        <v>1275.69331660583</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>819.64769553072597</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>42461</v>
       </c>
@@ -1586,10 +1569,10 @@
         <v>2018</v>
       </c>
       <c r="C65" s="3">
-        <v>1462.6511694785199</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>735.89568014705799</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>42491</v>
       </c>
@@ -1597,10 +1580,10 @@
         <v>2003</v>
       </c>
       <c r="C66" s="3">
-        <v>1325.81495098039</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>942.90266719745205</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>42491</v>
       </c>
@@ -1608,10 +1591,10 @@
         <v>2004</v>
       </c>
       <c r="C67" s="3">
-        <v>1372.70965189873</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>856.54830545774598</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>42491</v>
       </c>
@@ -1619,10 +1602,10 @@
         <v>2005</v>
       </c>
       <c r="C68" s="3">
-        <v>1260.92144396551</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>815.65686274509801</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>42491</v>
       </c>
@@ -1630,10 +1613,10 @@
         <v>2006</v>
       </c>
       <c r="C69" s="3">
-        <v>1326.55188679245</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>848.62257543103397</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>42491</v>
       </c>
@@ -1641,10 +1624,10 @@
         <v>2007</v>
       </c>
       <c r="C70" s="3">
-        <v>1328.21854967948</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>770.62869822485197</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>42491</v>
       </c>
@@ -1652,10 +1635,10 @@
         <v>2008</v>
       </c>
       <c r="C71" s="3">
-        <v>1307.98854813664</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>893.93318014705801</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>42491</v>
       </c>
@@ -1663,10 +1646,10 @@
         <v>2009</v>
       </c>
       <c r="C72" s="3">
-        <v>1275.869140625</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>794.06226325757495</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>42491</v>
       </c>
@@ -1674,10 +1657,10 @@
         <v>2010</v>
       </c>
       <c r="C73" s="3">
-        <v>1221.8229166666599</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>854.41591401734104</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>42491</v>
       </c>
@@ -1685,10 +1668,10 @@
         <v>2011</v>
       </c>
       <c r="C74" s="3">
-        <v>1179.37756849315</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>805.34853316326496</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>42491</v>
       </c>
@@ -1696,10 +1679,10 @@
         <v>2012</v>
       </c>
       <c r="C75" s="3">
-        <v>1273.7726151315701</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>805.32998991935403</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>42491</v>
       </c>
@@ -1707,10 +1690,10 @@
         <v>2013</v>
       </c>
       <c r="C76" s="3">
-        <v>1361.4132291666599</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>956.03920284431103</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>42491</v>
       </c>
@@ -1718,10 +1701,10 @@
         <v>2014</v>
       </c>
       <c r="C77" s="3">
-        <v>1308.3872195512799</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>830.74354383680497</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>42491</v>
       </c>
@@ -1729,10 +1712,10 @@
         <v>2015</v>
       </c>
       <c r="C78" s="3">
-        <v>1160.4137414383499</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>672.55675899621201</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>42491</v>
       </c>
@@ -1740,10 +1723,10 @@
         <v>2016</v>
       </c>
       <c r="C79" s="3">
-        <v>1347.4480149371</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>847.79886363636297</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>42491</v>
       </c>
@@ -1751,10 +1734,10 @@
         <v>2017</v>
       </c>
       <c r="C80" s="3">
-        <v>1489.3023097826001</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1098.4197168508199</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>42491</v>
       </c>
@@ -1762,10 +1745,10 @@
         <v>2018</v>
       </c>
       <c r="C81" s="3">
-        <v>1361.56444099378</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>883.10287921348299</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>42522</v>
       </c>
@@ -1773,10 +1756,10 @@
         <v>2003</v>
       </c>
       <c r="C82" s="3">
-        <v>1476.1610429447801</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1008.3602221385499</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>42522</v>
       </c>
@@ -1784,10 +1767,10 @@
         <v>2004</v>
       </c>
       <c r="C83" s="3">
-        <v>1460.36085838607</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1012.28618421052</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>42522</v>
       </c>
@@ -1795,10 +1778,10 @@
         <v>2005</v>
       </c>
       <c r="C84" s="3">
-        <v>1341.3334009740199</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>910.61595911949598</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>42522</v>
       </c>
@@ -1806,10 +1789,10 @@
         <v>2006</v>
       </c>
       <c r="C85" s="3">
-        <v>1481.0954741379301</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>987.41377314814804</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>42522</v>
       </c>
@@ -1817,10 +1800,10 @@
         <v>2007</v>
       </c>
       <c r="C86" s="3">
-        <v>1412.7515822784801</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>890.35863095238096</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>42522</v>
       </c>
@@ -1828,10 +1811,10 @@
         <v>2008</v>
       </c>
       <c r="C87" s="3">
-        <v>1452.69214794303</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>922.66156045751598</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>42522</v>
       </c>
@@ -1839,10 +1822,10 @@
         <v>2009</v>
       </c>
       <c r="C88" s="3">
-        <v>1323.3231488853501</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>877.44613970588205</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>42522</v>
       </c>
@@ -1850,10 +1833,10 @@
         <v>2010</v>
       </c>
       <c r="C89" s="3">
-        <v>1345.4713212025299</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>905.64215874233105</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>42522</v>
       </c>
@@ -1861,10 +1844,10 @@
         <v>2011</v>
       </c>
       <c r="C90" s="3">
-        <v>1304.4349449685501</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>825.8515625</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>42522</v>
       </c>
@@ -1872,10 +1855,10 @@
         <v>2012</v>
       </c>
       <c r="C91" s="3">
-        <v>1436.1556490384601</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>942.99589843750005</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>42522</v>
       </c>
@@ -1883,10 +1866,10 @@
         <v>2013</v>
       </c>
       <c r="C92" s="3">
-        <v>1417.7907436708799</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>982.348295454545</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>42522</v>
       </c>
@@ -1894,10 +1877,10 @@
         <v>2014</v>
       </c>
       <c r="C93" s="3">
-        <v>1297.0113824503301</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>833.07986111111097</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>42522</v>
       </c>
@@ -1905,10 +1888,10 @@
         <v>2015</v>
       </c>
       <c r="C94" s="3">
-        <v>1356.44768591772</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>822.32483057228899</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>42522</v>
       </c>
@@ -1916,10 +1899,10 @@
         <v>2016</v>
       </c>
       <c r="C95" s="3">
-        <v>1419.95234375</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1018.54975076687</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>42522</v>
       </c>
@@ -1927,10 +1910,10 @@
         <v>2017</v>
       </c>
       <c r="C96" s="3">
-        <v>1390.4746799698701</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>993.04940878378295</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>42522</v>
       </c>
@@ -1938,10 +1921,10 @@
         <v>2018</v>
       </c>
       <c r="C97" s="3">
-        <v>1412.4940390173399</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>950.661326142132</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>42552</v>
       </c>
@@ -1949,10 +1932,10 @@
         <v>2003</v>
       </c>
       <c r="C98" s="3">
-        <v>1670.68789308176</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1165.25306919642</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>42552</v>
       </c>
@@ -1960,10 +1943,10 @@
         <v>2004</v>
       </c>
       <c r="C99" s="3">
-        <v>1571.72666396103</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1136.0395710059099</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>42552</v>
       </c>
@@ -1971,10 +1954,10 @@
         <v>2005</v>
       </c>
       <c r="C100" s="3">
-        <v>1495.6972903481001</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1006.22567114093</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>42552</v>
       </c>
@@ -1982,10 +1965,10 @@
         <v>2006</v>
       </c>
       <c r="C101" s="3">
-        <v>1430.7733333333299</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1016.19997970779</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>42552</v>
       </c>
@@ -1993,10 +1976,10 @@
         <v>2007</v>
       </c>
       <c r="C102" s="3">
-        <v>1447.1401273885299</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>981.481231508875</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>42552</v>
       </c>
@@ -2004,10 +1987,10 @@
         <v>2008</v>
       </c>
       <c r="C103" s="3">
-        <v>1605.74258814102</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>979.72072784810098</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>42552</v>
       </c>
@@ -2015,10 +1998,10 @@
         <v>2009</v>
       </c>
       <c r="C104" s="3">
-        <v>1536.2676886792401</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1036.08229813664</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>42552</v>
       </c>
@@ -2026,10 +2009,10 @@
         <v>2010</v>
       </c>
       <c r="C105" s="3">
-        <v>1486.8832661290301</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1051.3528645833301</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>42552</v>
       </c>
@@ -2037,10 +2020,10 @@
         <v>2011</v>
       </c>
       <c r="C106" s="3">
-        <v>1494.3260350318401</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>955.08098323170702</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>42552</v>
       </c>
@@ -2048,10 +2031,10 @@
         <v>2012</v>
       </c>
       <c r="C107" s="3">
-        <v>1550.8803401898699</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1046.6980932203301</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>42552</v>
       </c>
@@ -2059,10 +2042,10 @@
         <v>2013</v>
       </c>
       <c r="C108" s="3">
-        <v>1595.9349767080701</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1125.9228766025601</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>42552</v>
       </c>
@@ -2070,10 +2053,10 @@
         <v>2014</v>
       </c>
       <c r="C109" s="3">
-        <v>1443.83000395569</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1063.5653409090901</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>42552</v>
       </c>
@@ -2081,10 +2064,10 @@
         <v>2015</v>
       </c>
       <c r="C110" s="3">
-        <v>1445.4613853503099</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>999.49498456790104</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>42552</v>
       </c>
@@ -2092,10 +2075,10 @@
         <v>2016</v>
       </c>
       <c r="C111" s="3">
-        <v>1686.6359848484799</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1091.6653196839</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>42552</v>
       </c>
@@ -2103,10 +2086,10 @@
         <v>2017</v>
       </c>
       <c r="C112" s="3">
-        <v>1472.8899739583301</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1016.0394425675599</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>42552</v>
       </c>
@@ -2114,10 +2097,10 @@
         <v>2018</v>
       </c>
       <c r="C113" s="3">
-        <v>1573.5058139534799</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1012.078125</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>42583</v>
       </c>
@@ -2125,10 +2108,10 @@
         <v>2003</v>
       </c>
       <c r="C114" s="3">
-        <v>1720.0806130573201</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1299.3226943597499</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>42583</v>
       </c>
@@ -2136,10 +2119,10 @@
         <v>2004</v>
       </c>
       <c r="C115" s="3">
-        <v>1685.89443108974</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1289.1514274691301</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>42583</v>
       </c>
@@ -2147,10 +2130,10 @@
         <v>2005</v>
       </c>
       <c r="C116" s="3">
-        <v>1511.2939967105201</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1034.2730654761899</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>42583</v>
       </c>
@@ -2158,10 +2141,10 @@
         <v>2006</v>
       </c>
       <c r="C117" s="3">
-        <v>1489.9947567114</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>947.38417968750002</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>42583</v>
       </c>
@@ -2169,10 +2152,10 @@
         <v>2007</v>
       </c>
       <c r="C118" s="3">
-        <v>1462.01209332191</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>945.06011146496803</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>42583</v>
       </c>
@@ -2180,10 +2163,10 @@
         <v>2008</v>
       </c>
       <c r="C119" s="3">
-        <v>1480.2689144736801</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>949.84641768292602</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>42583</v>
       </c>
@@ -2191,10 +2174,10 @@
         <v>2009</v>
       </c>
       <c r="C120" s="3">
-        <v>1477.1479301948</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>940.29125816993405</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>42583</v>
       </c>
@@ -2202,10 +2185,10 @@
         <v>2010</v>
       </c>
       <c r="C121" s="3">
-        <v>1637.51143036912</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1086.2358141447301</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>42583</v>
       </c>
@@ -2213,10 +2196,10 @@
         <v>2011</v>
       </c>
       <c r="C122" s="3">
-        <v>1370.55645529197</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>934.15604838709601</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>42583</v>
       </c>
@@ -2224,10 +2207,10 @@
         <v>2012</v>
       </c>
       <c r="C123" s="3">
-        <v>1401.0955882352901</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>957.15362903225798</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>42583</v>
       </c>
@@ -2235,10 +2218,10 @@
         <v>2013</v>
       </c>
       <c r="C124" s="3">
-        <v>1518.86698717948</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1018.37219827586</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>42583</v>
       </c>
@@ -2246,10 +2229,10 @@
         <v>2014</v>
       </c>
       <c r="C125" s="3">
-        <v>1432.91446834415</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>955.84980867346906</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>42583</v>
       </c>
@@ -2257,10 +2240,10 @@
         <v>2015</v>
       </c>
       <c r="C126" s="3">
-        <v>1512.0148237179401</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>963.35219594594503</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>42583</v>
       </c>
@@ -2268,10 +2251,10 @@
         <v>2016</v>
       </c>
       <c r="C127" s="3">
-        <v>1573.09927591463</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1018.63382711038</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>42583</v>
       </c>
@@ -2279,10 +2262,10 @@
         <v>2017</v>
       </c>
       <c r="C128" s="3">
-        <v>1580.7580492424199</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1008.42455357142</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>42583</v>
       </c>
@@ -2291,7 +2274,7 @@
       </c>
       <c r="C129" s="4"/>
     </row>
-    <row r="130" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>42614</v>
       </c>
@@ -2299,10 +2282,10 @@
         <v>2003</v>
       </c>
       <c r="C130" s="3">
-        <v>1545.3155208333301</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1153.3556170886</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>42614</v>
       </c>
@@ -2310,10 +2293,10 @@
         <v>2004</v>
       </c>
       <c r="C131" s="3">
-        <v>1664.1121504934199</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1163.21856398809</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>42614</v>
       </c>
@@ -2321,10 +2304,10 @@
         <v>2005</v>
       </c>
       <c r="C132" s="3">
-        <v>1483.2322635135099</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1139.8058320063601</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>42614</v>
       </c>
@@ -2332,10 +2315,10 @@
         <v>2006</v>
       </c>
       <c r="C133" s="3">
-        <v>1480.9208255597</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1023.47791666666</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>42614</v>
       </c>
@@ -2343,10 +2326,10 @@
         <v>2007</v>
       </c>
       <c r="C134" s="3">
-        <v>1294.1602678571401</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>896.07228915662597</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>42614</v>
       </c>
@@ -2354,10 +2337,10 @@
         <v>2008</v>
       </c>
       <c r="C135" s="3">
-        <v>1347.9581250000001</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>913.82903225806399</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>42614</v>
       </c>
@@ -2365,10 +2348,10 @@
         <v>2009</v>
       </c>
       <c r="C136" s="3">
-        <v>1298.0012019230701</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>841.89158950617195</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>42614</v>
       </c>
@@ -2376,10 +2359,10 @@
         <v>2010</v>
       </c>
       <c r="C137" s="3">
-        <v>1430.46416666666</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1019.95008389261</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>42614</v>
       </c>
@@ -2387,10 +2370,10 @@
         <v>2011</v>
       </c>
       <c r="C138" s="3">
-        <v>1338.43783482142</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>875.22487745097999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>42614</v>
       </c>
@@ -2398,10 +2381,10 @@
         <v>2012</v>
       </c>
       <c r="C139" s="3">
-        <v>1395.64859479865</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>943.569972826087</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>42614</v>
       </c>
@@ -2409,10 +2392,10 @@
         <v>2013</v>
       </c>
       <c r="C140" s="3">
-        <v>1392.3507056451599</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>997.83249999999998</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>42614</v>
       </c>
@@ -2420,10 +2403,10 @@
         <v>2014</v>
       </c>
       <c r="C141" s="3">
-        <v>1459.2386363636299</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>950.20773381294896</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>42614</v>
       </c>
@@ -2431,10 +2414,10 @@
         <v>2015</v>
       </c>
       <c r="C142" s="3">
-        <v>1344.99258814102</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>934.31077516233699</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>42614</v>
       </c>
@@ -2442,10 +2425,10 @@
         <v>2016</v>
       </c>
       <c r="C143" s="3">
-        <v>1392.9457831325301</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>961.46830357142801</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>42614</v>
       </c>
@@ -2453,10 +2436,10 @@
         <v>2017</v>
       </c>
       <c r="C144" s="3">
-        <v>1408.7804831288299</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>990.71856725146199</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>42614</v>
       </c>
@@ -2465,7 +2448,7 @@
       </c>
       <c r="C145" s="4"/>
     </row>
-    <row r="146" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>42644</v>
       </c>
@@ -2473,10 +2456,10 @@
         <v>2003</v>
       </c>
       <c r="C146" s="3">
-        <v>1292.8154709507</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1021.1027097902</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>42644</v>
       </c>
@@ -2484,10 +2467,10 @@
         <v>2004</v>
       </c>
       <c r="C147" s="3">
-        <v>1404.0861863057301</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>997.49597679640704</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>42644</v>
       </c>
@@ -2495,10 +2478,10 @@
         <v>2005</v>
       </c>
       <c r="C148" s="3">
-        <v>1219.3612068965499</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>918.38245033112503</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>42644</v>
       </c>
@@ -2506,10 +2489,10 @@
         <v>2006</v>
       </c>
       <c r="C149" s="3">
-        <v>1272.00681627516</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>916.77368630573199</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>42644</v>
       </c>
@@ -2517,10 +2500,10 @@
         <v>2007</v>
       </c>
       <c r="C150" s="3">
-        <v>1153.29217657342</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>804.75667425496601</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>42644</v>
       </c>
@@ -2528,10 +2511,10 @@
         <v>2008</v>
       </c>
       <c r="C151" s="3">
-        <v>1243.4375</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>791.67430449695098</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>42644</v>
       </c>
@@ -2539,10 +2522,10 @@
         <v>2009</v>
       </c>
       <c r="C152" s="3">
-        <v>1191.1433467741899</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>804.29480698529403</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>42644</v>
       </c>
@@ -2550,10 +2533,10 @@
         <v>2010</v>
       </c>
       <c r="C153" s="3">
-        <v>1247.01164215686</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>930.57793328220805</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>42644</v>
       </c>
@@ -2561,10 +2544,10 @@
         <v>2011</v>
       </c>
       <c r="C154" s="3">
-        <v>1099.70301418439</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>732.57456961077798</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>42644</v>
       </c>
@@ -2572,10 +2555,10 @@
         <v>2012</v>
       </c>
       <c r="C155" s="3">
-        <v>1109.0200320512799</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>803.19362207602296</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>42644</v>
       </c>
@@ -2583,10 +2566,10 @@
         <v>2013</v>
       </c>
       <c r="C156" s="3">
-        <v>1163.7327127659501</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>759.43255046583795</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>42644</v>
       </c>
@@ -2594,10 +2577,10 @@
         <v>2014</v>
       </c>
       <c r="C157" s="3">
-        <v>1304.8051658163199</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>809.00847630718897</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>42644</v>
       </c>
@@ -2605,10 +2588,10 @@
         <v>2015</v>
       </c>
       <c r="C158" s="3">
-        <v>1143.8049768518499</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>780.45285744862997</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>42644</v>
       </c>
@@ -2616,10 +2599,10 @@
         <v>2016</v>
       </c>
       <c r="C159" s="3">
-        <v>1365.82389705882</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>995.677734375</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>42644</v>
       </c>
@@ -2627,10 +2610,10 @@
         <v>2017</v>
       </c>
       <c r="C160" s="3">
-        <v>1227.2353316326501</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>955.95772058823502</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>42644</v>
       </c>
@@ -2639,7 +2622,7 @@
       </c>
       <c r="C161" s="4"/>
     </row>
-    <row r="162" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>42675</v>
       </c>
@@ -2647,10 +2630,10 @@
         <v>2003</v>
       </c>
       <c r="C162" s="3">
-        <v>1109.0398284313701</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>748.43854166666597</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>42675</v>
       </c>
@@ -2658,10 +2641,10 @@
         <v>2004</v>
       </c>
       <c r="C163" s="3">
-        <v>1172.5377083333301</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>787.59718351910794</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>42675</v>
       </c>
@@ -2669,10 +2652,10 @@
         <v>2005</v>
       </c>
       <c r="C164" s="3">
-        <v>1136.60304588607</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>766.42148437499998</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>42675</v>
       </c>
@@ -2680,10 +2663,10 @@
         <v>2006</v>
       </c>
       <c r="C165" s="3">
-        <v>1083.71544894366</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>800.90885416666595</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>42675</v>
       </c>
@@ -2691,10 +2674,10 @@
         <v>2007</v>
       </c>
       <c r="C166" s="3">
-        <v>1082.7636471518899</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>679.67556288819799</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>42675</v>
       </c>
@@ -2702,10 +2685,10 @@
         <v>2008</v>
       </c>
       <c r="C167" s="3">
-        <v>1028.69620253164</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>637.64215686274497</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>42675</v>
       </c>
@@ -2713,10 +2696,10 @@
         <v>2009</v>
       </c>
       <c r="C168" s="3">
-        <v>1141.06611328125</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>674.27241443452294</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>42675</v>
       </c>
@@ -2724,10 +2707,10 @@
         <v>2010</v>
       </c>
       <c r="C169" s="3">
-        <v>1096.68052279874</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>719.96626838235295</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>42675</v>
       </c>
@@ -2735,10 +2718,10 @@
         <v>2011</v>
       </c>
       <c r="C170" s="3">
-        <v>993.90100931677</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>582.73487463662696</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>42675</v>
       </c>
@@ -2746,10 +2729,10 @@
         <v>2012</v>
       </c>
       <c r="C171" s="3">
-        <v>954.37155172413702</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>660.80995973926304</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>42675</v>
       </c>
@@ -2757,10 +2740,10 @@
         <v>2013</v>
       </c>
       <c r="C172" s="3">
-        <v>1013.55300632911</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>669.50753837719299</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>42675</v>
       </c>
@@ -2768,10 +2751,10 @@
         <v>2014</v>
       </c>
       <c r="C173" s="3">
-        <v>1032.10505756578</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>639.20238095238096</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>42675</v>
       </c>
@@ -2779,10 +2762,10 @@
         <v>2015</v>
       </c>
       <c r="C174" s="3">
-        <v>1147.55136846405</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>754.57488567073096</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>42675</v>
       </c>
@@ -2790,10 +2773,10 @@
         <v>2016</v>
       </c>
       <c r="C175" s="3">
-        <v>1229.1523203592801</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>749.48032407407402</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>42675</v>
       </c>
@@ -2801,10 +2784,10 @@
         <v>2017</v>
       </c>
       <c r="C176" s="3">
-        <v>1167.31892857142</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>800.32691062176104</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>42675</v>
       </c>
@@ -2813,7 +2796,7 @@
       </c>
       <c r="C177" s="4"/>
     </row>
-    <row r="178" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>42705</v>
       </c>
@@ -2821,10 +2804,10 @@
         <v>2003</v>
       </c>
       <c r="C178" s="3">
-        <v>1199.2425314465399</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>746.27599597953201</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>42705</v>
       </c>
@@ -2832,10 +2815,10 @@
         <v>2004</v>
       </c>
       <c r="C179" s="3">
-        <v>1113.7371386054399</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>735.74891493055497</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>42705</v>
       </c>
@@ -2843,10 +2826,10 @@
         <v>2005</v>
       </c>
       <c r="C180" s="3">
-        <v>1160.7684004934199</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>740.93514683734895</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>42705</v>
       </c>
@@ -2854,10 +2837,10 @@
         <v>2006</v>
       </c>
       <c r="C181" s="3">
-        <v>1099.7348726114601</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>781.67482311320703</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>42705</v>
       </c>
@@ -2865,10 +2848,10 @@
         <v>2007</v>
       </c>
       <c r="C182" s="3">
-        <v>1087.2403085443</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>654.07702323717899</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>42705</v>
       </c>
@@ -2876,10 +2859,10 @@
         <v>2008</v>
       </c>
       <c r="C183" s="3">
-        <v>1040.6798427152301</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>686.79636101973597</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>42705</v>
       </c>
@@ -2887,10 +2870,10 @@
         <v>2009</v>
       </c>
       <c r="C184" s="3">
-        <v>1117.9382961783399</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>706.21984011627899</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>42705</v>
       </c>
@@ -2898,10 +2881,10 @@
         <v>2010</v>
       </c>
       <c r="C185" s="3">
-        <v>1025.6827531645499</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>683.23304115853603</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>42705</v>
       </c>
@@ -2909,10 +2892,10 @@
         <v>2011</v>
       </c>
       <c r="C186" s="3">
-        <v>1179.90941584967</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>770.80625982704396</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>42705</v>
       </c>
@@ -2920,10 +2903,10 @@
         <v>2012</v>
       </c>
       <c r="C187" s="3">
-        <v>1048.3622159090901</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>789.46257267441797</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>42705</v>
       </c>
@@ -2931,10 +2914,10 @@
         <v>2013</v>
       </c>
       <c r="C188" s="3">
-        <v>1112.8309928797401</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>648.828725961538</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>42705</v>
       </c>
@@ -2942,10 +2925,10 @@
         <v>2014</v>
       </c>
       <c r="C189" s="3">
-        <v>1053.9437893081699</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>643.02426242236004</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>42705</v>
       </c>
@@ -2953,10 +2936,10 @@
         <v>2015</v>
       </c>
       <c r="C190" s="3">
-        <v>1209.7705696202499</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>734.86603180473298</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>42705</v>
       </c>
@@ -2964,10 +2947,10 @@
         <v>2016</v>
       </c>
       <c r="C191" s="3">
-        <v>1246.4109563253</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>717.17890188547403</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>42705</v>
       </c>
@@ -2975,10 +2958,10 @@
         <v>2017</v>
       </c>
       <c r="C192" s="3">
-        <v>1116.1179142441799</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+        <v>771.85974482248503</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>42705</v>
       </c>

</xml_diff>